<commit_message>
QA and update files to console
</commit_message>
<xml_diff>
--- a/console/Networking/iaas-network/pipMixinsXlsx/bgpipMove.xlsx
+++ b/console/Networking/iaas-network/pipMixinsXlsx/bgpipMove.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GTCOM\JD\!!Workspace\1811-14_HB\console-EN_Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ch" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -624,18 +629,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>If public IP to be upgraded is under associated state (IP in arrears or due does not participate in switching activities), we recommend you release the association between public IP and cloud resources to ensure the stability of upgrade process.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Upgrading Steps</t>
     </r>
   </si>
@@ -672,18 +665,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The original IP will have an extended retention period of 2 months from now on. The functions of renewal, automatic renewal, bandwidth modification of the original IP will be disabled during this period, and other functions will be retained, so that you can switch the IP associated to your business stably and safely during the retention period.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>When the extension of the original IP retention period is about to expire, the customer service staff of JD Cloud official website will notify you to switch IP as soon as possible by phone calls, SMS, intra-website messages or emails, so as not to delay the normal use of your businesses.</t>
     </r>
   </si>
@@ -708,18 +689,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>After confirming that there is no problem with the association between the new IP and your businesses, click the delete button with a red package identifier and delete the original IP to receive the coupon rewards.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Coupon Rewarding Rules</t>
     </r>
   </si>
@@ -756,18 +725,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Pay by configuration billing IP will be issued an equivalent coupon of 2 months current bandwidth use fee; pay by consumption billing IP will be issued an equivalent coupon of 2 months retention fee; for monthly package billing method, the new IP expiration time after replication is equal to the number of remaining months of the original IP (in special cases, the expiration time of the new IP will be less than that of the original IP, and the expiration time will be replenished in the form of equivalent coupon).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Original IP Deletion Stage</t>
     </r>
   </si>
@@ -781,18 +738,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Users who actively delete the original IP with red package identifier can receive coupons with fixed amount.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If you have any questions during IP switching, please call customer service at 4006151212 (7</t>
     </r>
   </si>
   <si>
@@ -825,6 +770,173 @@
   </si>
   <si>
     <t>In order to ensure that JD Cloud can provide you stable, reliable, secure cloud computing service, JD Cloud will conduct BGP IP upgrade service. JD Cloud products purchased after upgrade will all be new North China BGP IP, and existing IP will also be switched for upgrade. You can click **One Click Replication** on Public IP List page to participate this IP upgrade activity and get corresponding rewards. See the following rules for IP upgrade rewards and the arrangement of IP switching</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>The original IP will have an extended retention period of 2 months from now on. The functions of renewal, automatic renewal, bandwidth modification of the original IP will be disabled during this period, and other functions will be retained, so that you can switch the IP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> associated with your cloud resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> stably and safely during the retention period.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If public IP to be upgraded is under associated state (IP in arrears or due </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> not participate in switching activities), we recommend you release the association between public IP and cloud resources to ensure the stability of upgrade process.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After confirming that there is no problem with the association between the new IP and your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cloud resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, click the delete button with a red package identifier and delete the original IP to receive the coupon rewards.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The IP type paid by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> configuration billing will be issued an equivalent coupon of 2 months current bandwidth use fee;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the IP type paid by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>consumption billing will be issued an equivalent coupon of 2 months retention fee; for monthly package billing method, the new IP expiration time after replication is equal to the number of remaining months of the original IP (in special cases, the expiration time of the new IP will be less than that of the original IP, and the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> shortage of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expiration time will be replenished in the form of equivalent coupon).</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you have any questions during IP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">upgration and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>switching, please call customer service at 4006151212 (7</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -832,7 +944,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -845,6 +957,13 @@
       <name val="Arial"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -875,7 +994,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1214,17 +1333,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="23.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.21875" customWidth="1"/>
-    <col min="3" max="3" width="74.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.1796875" customWidth="1"/>
+    <col min="3" max="3" width="74.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1354,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1365,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1376,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1265,10 +1384,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1398,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1287,10 +1406,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1298,10 +1417,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1309,10 +1428,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1320,10 +1439,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1331,10 +1450,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1342,10 +1461,10 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1353,10 +1472,10 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1364,10 +1483,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1375,10 +1494,10 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1386,10 +1505,10 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1397,10 +1516,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1408,10 +1527,10 @@
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1419,10 +1538,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1430,10 +1549,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1441,10 +1560,10 @@
         <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1452,10 +1571,10 @@
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1463,10 +1582,10 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1474,12 +1593,13 @@
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <ignoredErrors>
     <ignoredError sqref="A1:B23" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>